<commit_message>
refactoring and excels sheet generated
</commit_message>
<xml_diff>
--- a/data/output-cities.xlsx
+++ b/data/output-cities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shernaliew/CZ2001-Lab4B/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherna\Documents\CZ2001-Lab4B\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23DD148-EDAC-9349-9BB3-74314064B4BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAE693E-E428-40B5-BCAB-31C7F14C5C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>No. of Cities</t>
   </si>
@@ -33,36 +33,6 @@
   </si>
   <si>
     <t>Fraction of Max. Edges</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
 </sst>
 </file>
@@ -98,8 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,7 +91,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -172,7 +143,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Experiment 1'!$C$1</c:f>
+              <c:f>'Experiment 1'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -260,7 +231,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Experiment 1'!$C$2:$C$11</c:f>
+              <c:f>'Experiment 1'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -300,7 +271,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9BD5-3A45-A95E-8FC04AB0788E}"/>
+              <c16:uniqueId val="{00000000-87F4-43AC-BC5A-0BF290ED904D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -312,11 +283,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="563590223"/>
-        <c:axId val="563591855"/>
+        <c:axId val="1033485168"/>
+        <c:axId val="1172382368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="563590223"/>
+        <c:axId val="1033485168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -337,6 +308,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Number of Cities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -403,12 +399,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563591855"/>
+        <c:crossAx val="1172382368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="563591855"/>
+        <c:axId val="1172382368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,6 +424,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Average Execution Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -465,7 +516,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563590223"/>
+        <c:crossAx val="1033485168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -477,6 +528,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -524,7 +606,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -624,9 +706,10 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Experiment 2'!$B$2:$B$11</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
@@ -656,10 +739,10 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -703,7 +786,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8AFD-5C48-8ACE-1EC5CD406F2F}"/>
+              <c16:uniqueId val="{00000000-9101-43E6-B1B5-D70EA0B41AF1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -715,11 +798,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="508241839"/>
-        <c:axId val="508430031"/>
+        <c:axId val="1084458640"/>
+        <c:axId val="1087628704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="508241839"/>
+        <c:axId val="1084458640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,6 +822,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Fraction</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-SG" baseline="0"/>
+                  <a:t> of Maximum Number of Edges for 1000 cities</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-SG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -775,12 +918,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508430031"/>
+        <c:crossAx val="1087628704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="508430031"/>
+        <c:axId val="1087628704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,6 +943,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Average Execution Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -837,7 +1035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508241839"/>
+        <c:crossAx val="1084458640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -849,6 +1047,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2010,22 +2239,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8124984-F499-2540-A24D-56322CA0830F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEFA1DBD-E134-4875-BA89-D391004A69CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2051,22 +2280,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE97D5CD-559B-2642-AED6-8C4069380C32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E57629F5-2924-4B99-8C65-B09CA5CEFF66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2384,132 +2613,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
         <v>2475</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1.9923529999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
       <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
         <v>9950</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1.3188039999999995E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
       <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
         <v>22425</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1.2545289999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>400</v>
       </c>
       <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
         <v>39900</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1.5200379999999993E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
       <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
         <v>62375</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1.1474479999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>600</v>
       </c>
       <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
         <v>89850</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1.0630830000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>700</v>
       </c>
       <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
         <v>122325</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1.4332349999999995E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>800</v>
       </c>
       <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
         <v>159800</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1.4894529999999996E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>900</v>
       </c>
       <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
         <v>202275</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1.6720460000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000</v>
       </c>
       <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
         <v>249750</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1.5918759999999994E-2</v>
       </c>
     </row>
@@ -2524,12 +2786,12 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2543,12 +2805,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2" s="1">
+        <v>0.1</v>
       </c>
       <c r="C2">
         <v>49950</v>
@@ -2557,12 +2819,12 @@
         <v>3.4444889999999985E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3" s="1">
+        <v>0.2</v>
       </c>
       <c r="C3">
         <v>99900</v>
@@ -2571,12 +2833,12 @@
         <v>2.7497500000000005E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4" s="1">
+        <v>0.3</v>
       </c>
       <c r="C4">
         <v>149850</v>
@@ -2585,12 +2847,12 @@
         <v>2.5992500000000009E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5" s="1">
+        <v>0.4</v>
       </c>
       <c r="C5">
         <v>199800</v>
@@ -2599,12 +2861,12 @@
         <v>1.9060609999999995E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
+      <c r="B6" s="1">
+        <v>0.5</v>
       </c>
       <c r="C6">
         <v>249750</v>
@@ -2613,12 +2875,12 @@
         <v>2.1375380000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
+      <c r="B7" s="1">
+        <v>0.6</v>
       </c>
       <c r="C7">
         <v>299700</v>
@@ -2627,12 +2889,12 @@
         <v>1.3762500000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
+      <c r="B8" s="1">
+        <v>0.7</v>
       </c>
       <c r="C8">
         <v>349650</v>
@@ -2641,12 +2903,12 @@
         <v>8.9863200000000008E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1000</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
+      <c r="B9" s="1">
+        <v>0.8</v>
       </c>
       <c r="C9">
         <v>399600</v>
@@ -2655,12 +2917,12 @@
         <v>8.720710000000003E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1000</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
+      <c r="B10" s="1">
+        <v>0.9</v>
       </c>
       <c r="C10">
         <v>449550</v>
@@ -2669,12 +2931,12 @@
         <v>5.5344400000000007E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
+      <c r="B11" s="1">
+        <v>1</v>
       </c>
       <c r="C11">
         <v>499500</v>

</xml_diff>